<commit_message>
recorrer arbol de categorias
</commit_message>
<xml_diff>
--- a/salida.xlsx
+++ b/salida.xlsx
@@ -413,7 +413,7 @@
       <row>12</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2095500" cy="1809750"/>
+    <ext cx="2095500" cy="1724025"/>
     <pic>
       <nvPicPr>
         <cNvPr id="12" name="Image 12" descr="Picture"/>
@@ -538,7 +538,7 @@
       <row>17</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2095500" cy="1809750"/>
+    <ext cx="2095500" cy="1724025"/>
     <pic>
       <nvPicPr>
         <cNvPr id="17" name="Image 17" descr="Picture"/>
@@ -563,7 +563,7 @@
       <row>18</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="2095500" cy="1809750"/>
+    <ext cx="2095500" cy="1724025"/>
     <pic>
       <nvPicPr>
         <cNvPr id="18" name="Image 18" descr="Picture"/>
@@ -1118,7 +1118,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB29"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
@@ -1175,14 +1175,24 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Catálogos vigentes</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Imusa</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>Batería 10 Piezas Antiadherente Gris Talent</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Batería 10 Piezas Antiadherente Gris Talent</t>
-        </is>
-      </c>
       <c r="G2" t="inlineStr">
         <is>
           <t>199.900</t>
@@ -1190,454 +1200,906 @@
       </c>
     </row>
     <row r="3" ht="160" customHeight="1">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Catálogos vigentes</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Campaña Regalos</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Hasta $199.900</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Hogar y Decorción Hasta $199.900</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Bateria 6 Piezas + Utensilio Gris Talent</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>149.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="160" customHeight="1">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Catálogos vigentes</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Especial de Madres</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Cocina para Mamá</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>Batería 10 Piezas Prograde Negra T-fal</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Batería 10 Piezas Prograde Negra T-fal</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>599.900</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="160" customHeight="1">
-      <c r="C4" t="inlineStr">
+    <row r="5" ht="160" customHeight="1">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Catálogos vigentes</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Campaña Regalos</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Hasta $99.900</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Hogar y Decorción Hasta $99.900</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
         <is>
           <t>Cuchillo X5 Unidades +Tijera Con Taco Madera</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Cuchillo X5 Unidades +Tijera Con Taco Madera</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>34.900</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="160" customHeight="1">
-      <c r="D5" t="inlineStr">
+    <row r="6" ht="160" customHeight="1">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Baño, Cocina y Aseo</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Ollas y Utensilios</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Tablas, Ralladores y Cortadores de Verduras</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>Tabla Picar 40x25Cm + Cuchillo X2Und 20 Y 12Cm Acero Inoxidable</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Tabla Picar 40x25Cm + Cuchillo X2Und 20 Y 12Cm Acero Inoxidable</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>29.900</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="160" customHeight="1">
-      <c r="E6" t="inlineStr">
+    <row r="7" ht="160" customHeight="1">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Catálogos vigentes</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Campaña Regalos</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Hasta $99.900</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Hogar y Decorción Hasta $99.900</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Cafetera 350Ml Presión Negra Home Collection</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>14.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="160" customHeight="1">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Baño, Cocina y Aseo</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Ollas y Utensilios</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Ollas y Baterias de Cocina</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Baterías de cocina</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Bateria 10 Piezas Acero Inoxidable</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>179.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="160" customHeight="1">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Baño, Cocina y Aseo</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Ollas y Utensilios</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Sartenes, Planchas y Woks</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Sartén X3Und 20 24 Y 32 Cm Antiadherente Negro</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>42.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="160" customHeight="1">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Catálogos vigentes</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Imusa</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Sartén Para Arepas IMUSA Smart Antiadherente</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>26.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="160" customHeight="1">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Catálogos vigentes</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Campaña Regalos</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Hasta $99.900</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Hogar y Decorción Hasta $99.900</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
         <is>
           <t>Batería 7 Piezas Acero Tapa Vidrio</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Batería 7 Piezas Acero Tapa Vidrio</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>136.900</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="160" customHeight="1">
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Sartén X3Und 20 24 Y 32 Cm Antiadherente Negro</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
+    <row r="12" ht="160" customHeight="1">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Baño, Cocina y Aseo</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Ollas y Utensilios</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Ollas y Baterias de Cocina</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Baterías de cocina</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Batería 11 Piezas L39135 Aliada</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>189.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="160" customHeight="1">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Baño, Cocina y Aseo</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Ollas y Utensilios</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Tablas, Ralladores y Cortadores de Verduras</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Tabla en Bambu de 36 x 24 cm</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>19.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="160" customHeight="1">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Baño, Cocina y Aseo</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Ollas y Utensilios</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Refractarias, Moldes y Utensilios de Repostería</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Refractarias y Moldes</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Recipiente x6 Unidades 0.32-0.8-0.37-0.64-1.05 -1.5Lt Tapa</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>89.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="160" customHeight="1">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Baño, Cocina y Aseo</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Ollas y Utensilios</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Utensilios de Cocina</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Otros Utensilios de Cocina</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Portahuevos gallina rejilla cromado</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>29.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="160" customHeight="1">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Baño, Cocina y Aseo</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Ollas y Utensilios</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Ollas y Baterias de Cocina</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Baterías de cocina</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Bateria Antiadherente De 7 Piezas Con Tapas En Vidrio</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>109.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="160" customHeight="1">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Baño, Cocina y Aseo</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Ollas y Utensilios</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Utensilios de Cocina</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Otros Utensilios de Cocina</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Molde Arepa - Patacón Casa Bonita</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>10.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="160" customHeight="1">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Catálogos vigentes</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Imusa</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Chocolatera de 2 Litro con Tapa Roja</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>34.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="160" customHeight="1">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Catálogos vigentes</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Imusa</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Batería 12 Piezas Gris Antiadherente Talent</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>244.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="160" customHeight="1">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Baño, Cocina y Aseo</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Ollas y Utensilios</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Sartenes, Planchas y Woks</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Parrilla asar arepas</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>24.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="160" customHeight="1">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Baño, Cocina y Aseo</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Ollas y Utensilios</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Ollas y Baterias de Cocina</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Baterías de cocina</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Batería Antiadherente De 10 Piezas</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>219.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="160" customHeight="1">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Catálogos vigentes</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Imusa</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Sartén 20cm Antiadherente Con Tapa Vidrio Talent</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
         <is>
           <t>42.900</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="160" customHeight="1">
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Cafetera 350Ml Presión Negra Home Collection</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>14.900</t>
-        </is>
-      </c>
-    </row>
-    <row r="9" ht="160" customHeight="1">
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Bateria 10 Piezas Acero Inoxidable</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>179.900</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Bateria de 10 Piezas en Acero Inoxidable</t>
-        </is>
-      </c>
-    </row>
-    <row r="10" ht="160" customHeight="1">
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Batería 11 Piezas L39135 Aliada</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>189.900</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>Batería 11 Piezas L39135 Aliada</t>
-        </is>
-      </c>
-    </row>
-    <row r="11" ht="160" customHeight="1">
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Tabla en Bambu de 36 x 24 cm</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
+    <row r="23" ht="160" customHeight="1">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Baño, Cocina y Aseo</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Ollas y Utensilios</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Utensilios de Cocina</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Coladores y Centrífugas</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Colador 16Cm Mango Negro</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
         <is>
           <t>19.900</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Tabla en Bambu de 36 x 24 cm</t>
-        </is>
-      </c>
-    </row>
-    <row r="12" ht="160" customHeight="1">
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Molde Arepa - Patacón Casa Bonita</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>10.900</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>Molde Arepa - Patacón Casa Bonita</t>
-        </is>
-      </c>
-    </row>
-    <row r="13" ht="160" customHeight="1">
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Sartén Para Arepas IMUSA Smart Antiadherente</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>26.900</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>Sartén Para Arepas IMUSA Smart Antiadherente</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="160" customHeight="1">
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Chocolatera de 2 Litro con Tapa Roja</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>34.900</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>Chocolatera de 2 Litro con Tapa Roja</t>
-        </is>
-      </c>
-    </row>
-    <row r="15" ht="160" customHeight="1">
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Bateria Antiadherente De 7 Piezas Con Tapas En Vidrio</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>109.900</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>Bateria Antiadherente De 7 Piezas Con Tapas En Vidrio</t>
-        </is>
-      </c>
-    </row>
-    <row r="16" ht="160" customHeight="1">
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Batería Antiadherente De 10 Piezas</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>219.900</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>Batería Antiadherente De 10 Piezas</t>
-        </is>
-      </c>
-    </row>
-    <row r="17" ht="160" customHeight="1">
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Sartén 20cm Antiadherente Con Tapa Vidrio Talent</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>41.900</t>
-        </is>
-      </c>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>Sartén 20cm Antiadherente Con Tapa Vidrio Talent</t>
-        </is>
-      </c>
-    </row>
-    <row r="18" ht="160" customHeight="1">
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Portahuevos gallina rejilla cromado</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>29.900</t>
-        </is>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>Portahuevos Gallina Rejilla Cromado</t>
-        </is>
-      </c>
-    </row>
-    <row r="19" ht="160" customHeight="1">
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Batería 12 Piezas Gris Antiadherente Talent</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>244.900</t>
-        </is>
-      </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>Batería 12 Piezas Gris Antiadherente Talent</t>
-        </is>
-      </c>
-    </row>
-    <row r="20" ht="160" customHeight="1">
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Recipiente x6 Unidades 0.32-0.8-0.37-0.64-1.05 -1.5Lt Tapa</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
+    </row>
+    <row r="24" ht="160" customHeight="1">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Catálogos vigentes</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Imusa</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Batería 7 piezas IMUSA Talent Antiadherente</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>184.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="160" customHeight="1">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Baño, Cocina y Aseo</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Ollas y Utensilios</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Utensilios de Cocina</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Otros Utensilios de Cocina</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Espumador De Leche Negro</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>16.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" ht="160" customHeight="1">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Baño, Cocina y Aseo</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Ollas y Utensilios</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Ollas y Baterias de Cocina</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Baterías de cocina</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Batería Antiadherente De 5 Piezas Con Tapas De Vidrio</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>104.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="160" customHeight="1">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Catálogos vigentes</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Especial de Madres</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Cocina para Mamá</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Bateria 9 Piezas Acero Ring Roja</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>249.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="160" customHeight="1">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Catálogos vigentes</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Imusa</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Espátula Imusa Esencial Negro</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>6.900</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" ht="160" customHeight="1">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Ollas y Utencilios</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Catálogos vigentes</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Imusa</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Plancha 27cm Cuadrada Talent</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
         <is>
           <t>89.900</t>
         </is>
       </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>Recipiente x6 Unidades 0.32-0.8-0.37-0.64-1.05 -1.5Lt Tapa</t>
-        </is>
-      </c>
-    </row>
-    <row r="21" ht="160" customHeight="1">
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Bateria 9 Piezas Acero Ring Roja</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>249.900</t>
-        </is>
-      </c>
-      <c r="T21" t="inlineStr">
-        <is>
-          <t>Bateria 9 Piezas Acero Ring Roja</t>
-        </is>
-      </c>
-    </row>
-    <row r="22" ht="160" customHeight="1">
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Pinza Acero 30Cm</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>14.900</t>
-        </is>
-      </c>
-      <c r="U22" t="inlineStr">
-        <is>
-          <t>Pinza Acero 30Cm</t>
-        </is>
-      </c>
-    </row>
-    <row r="23" ht="160" customHeight="1">
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Batería Antiadherente De 5 Piezas Con Tapas De Vidrio</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>104.900</t>
-        </is>
-      </c>
-      <c r="V23" t="inlineStr">
-        <is>
-          <t>Batería Antiadherente De 5 Piezas Con Tapas De Vidrio</t>
-        </is>
-      </c>
-    </row>
-    <row r="24" ht="160" customHeight="1">
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Colador 16Cm Mango Negro</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>19.900</t>
-        </is>
-      </c>
-      <c r="W24" t="inlineStr">
-        <is>
-          <t>Colador 16Cm Mango Negro</t>
-        </is>
-      </c>
-    </row>
-    <row r="25" ht="160" customHeight="1">
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Plancha 27cm Cuadrada Talent</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>84.900</t>
-        </is>
-      </c>
-      <c r="X25" t="inlineStr">
-        <is>
-          <t>Plancha 27cm Cuadrada Talent</t>
-        </is>
-      </c>
-    </row>
-    <row r="26" ht="160" customHeight="1">
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Batería 7 piezas IMUSA Talent Antiadherente</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>184.900</t>
-        </is>
-      </c>
-      <c r="Y26" t="inlineStr">
-        <is>
-          <t>Batería 7 piezas IMUSA Talent Antiadherente</t>
-        </is>
-      </c>
-    </row>
-    <row r="27" ht="160" customHeight="1">
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Parrilla asar arepas</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>24.900</t>
-        </is>
-      </c>
-      <c r="Z27" t="inlineStr">
-        <is>
-          <t>Parrilla para Asar</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Espumador De Leche Negro</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>16.900</t>
-        </is>
-      </c>
-      <c r="AA28" t="inlineStr">
-        <is>
-          <t>Espumador De Leche Negro</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>Espátula Imusa Esencial Negro</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>6.900</t>
-        </is>
-      </c>
-      <c r="AB29" t="inlineStr">
-        <is>
-          <t>Espátula Imusa Esencial Negro</t>
-        </is>
-      </c>
-    </row>
+    </row>
+    <row r="30" ht="160" customHeight="1"/>
+    <row r="31" ht="160" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>